<commit_message>
Rename gauss-woc.tex to gauss-woc.sty
</commit_message>
<xml_diff>
--- a/expl3-refactor/gauss-macros.xlsx
+++ b/expl3-refactor/gauss-macros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/LaTeX/playground/gauss-matrix/expl3-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF533C99-855D-C044-9C61-FB142DA282E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8660444B-C443-3647-86C5-9478033BD0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{1189B7FD-FD26-8948-9152-87F43A6E616A}"/>
   </bookViews>
@@ -465,9 +465,6 @@
     <t>g@cbox#1#2#3</t>
   </si>
   <si>
-    <t>#1,#2 are gfloats, #3 is math material;  "#3 is put into an hbox which is at the point (#1,#2). The box will be vertically aligned to #2 (i.e., the math axis of #3 will be at height #2), and horizontally start at #1."</t>
-  </si>
-  <si>
     <t>#1,#2 are gfloats, #3 is math material; "Here, #3 will be centered horizontally to #1, whereas #2 denotes the height of the label's bottom."</t>
   </si>
   <si>
@@ -574,6 +571,9 @@
   </si>
   <si>
     <t>All arguments are gfloats; This macro draws a line from (#1,#2) to (#1,#3) using \put (TYPO IN DOCS: not (#1,#2) to (#2,#3)!)</t>
+  </si>
+  <si>
+    <t>#1,#2 are gfloats (more specifially: #1 is the x coordiante and #2 the y-coord), #3 is math material;  "#3 is put into an hbox which is at the point (#1,#2). The box will be vertically aligned to #2 (i.e., the math axis of #3 will be at height #2), and horizontally start at #1."</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1005,7 @@
         <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>40</v>
@@ -1019,10 +1019,10 @@
         <v>58</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>114</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>115</v>
@@ -1331,7 +1331,7 @@
         <v>129</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>120</v>
@@ -1392,12 +1392,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="108" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>120</v>
@@ -1408,7 +1408,7 @@
         <v>141</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>120</v>
@@ -1416,10 +1416,10 @@
     </row>
     <row r="52" spans="1:3" ht="108" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>120</v>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="53" spans="1:3" ht="180" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>120</v>
@@ -1438,43 +1438,43 @@
     </row>
     <row r="54" spans="1:3" ht="108" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="108" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>120</v>
@@ -1482,68 +1482,68 @@
     </row>
     <row r="59" spans="1:3" ht="180" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="162" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="72" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="288" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="72" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="36" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>39</v>
@@ -1551,13 +1551,13 @@
     </row>
     <row r="70" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1612,7 +1612,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>